<commit_message>
Added bangla in Author and Publisher
</commit_message>
<xml_diff>
--- a/book_rental/management/commands/uploads/publisher_upload.xlsx
+++ b/book_rental/management/commands/uploads/publisher_upload.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="20">
   <si>
     <t>code</t>
   </si>
@@ -19,9 +19,18 @@
     <t>publisher name</t>
   </si>
   <si>
+    <t>publisher name bn</t>
+  </si>
+  <si>
     <t>publisher description</t>
   </si>
   <si>
+    <t>publisher description bn</t>
+  </si>
+  <si>
+    <t>show bn</t>
+  </si>
+  <si>
     <t>publisher image</t>
   </si>
   <si>
@@ -32,6 +41,9 @@
   </si>
   <si>
     <t>Onno Prokashoni</t>
+  </si>
+  <si>
+    <t>মা আমার চোখের আলো</t>
   </si>
   <si>
     <t>adasdas</t>
@@ -65,20 +77,31 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="19.0"/>
+      <color rgb="FF444546"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,11 +115,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -140,107 +166,170 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>